<commit_message>
Updated Engine module to accommodate new GAMs model input and output file format.
</commit_message>
<xml_diff>
--- a/GamsResources/A-n6-k3-output-multi-vartemp-v2.2.xlsx
+++ b/GamsResources/A-n6-k3-output-multi-vartemp-v2.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yousuf\Eclipse  Workspace\OptEngineV3\GamsResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DFC020E-D304-4736-B696-324055360DFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7774D0A5-DF43-456E-8174-500B266F7AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4125" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{B1027DC1-41D9-4A09-9731-1676AB10685C}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{B1027DC1-41D9-4A09-9731-1676AB10685C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="36">
   <si>
     <t>Customers Demands:</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>Rank</t>
+  </si>
+  <si>
+    <t>03f808cdd997cee9</t>
+  </si>
+  <si>
+    <t>551d181c465cf86f</t>
+  </si>
+  <si>
+    <t>dummyTruck1</t>
+  </si>
+  <si>
+    <t>dummyTruck2</t>
   </si>
 </sst>
 </file>
@@ -487,18 +499,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE21476-BA80-4B0A-A345-8A1CCC0C7E6B}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -509,7 +521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -520,7 +532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -528,7 +540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -536,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -547,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -555,22 +567,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -586,8 +598,10 @@
       <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -604,9 +618,1003 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -839,15 +1847,502 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321FB39D-EE28-450E-A089-6B3309088C59}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D3">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E3">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D4">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E4">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D5">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E5">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D6">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E6">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>3.6444595271084532</v>
+      </c>
+      <c r="D7">
+        <v>5.6000608517325157</v>
+      </c>
+      <c r="E7">
+        <v>2.8058597983326381</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D8">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E8">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D9">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E9">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D10">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E10">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>3.2430985182082441</v>
+      </c>
+      <c r="D11">
+        <v>4.1200858108334959</v>
+      </c>
+      <c r="E11">
+        <v>2.7590612108253496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>3.5539162451403254</v>
+      </c>
+      <c r="D12">
+        <v>5.1916063476149779</v>
+      </c>
+      <c r="E12">
+        <v>2.7746264350228187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D13">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E13">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D14">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E14">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D15">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E15">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <v>3.4693316158731622</v>
+      </c>
+      <c r="D16">
+        <v>4.8536708963489748</v>
+      </c>
+      <c r="E16">
+        <v>2.7563818887307363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D17">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E17">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D18">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E18">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>3.2430985182082441</v>
+      </c>
+      <c r="D19">
+        <v>4.1200858108334959</v>
+      </c>
+      <c r="E19">
+        <v>2.7590612108253496</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20">
+        <v>3.643901643922447</v>
+      </c>
+      <c r="D20">
+        <v>5.5933116265477993</v>
+      </c>
+      <c r="E20">
+        <v>2.8040145872455757</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D21">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E21">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D22">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E22">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>3.5527263028024261</v>
+      </c>
+      <c r="D23">
+        <v>5.1779290554634585</v>
+      </c>
+      <c r="E23">
+        <v>2.7706365253248637</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D24">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E24">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D25">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E25">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D26">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E26">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>3.4682230888395553</v>
+      </c>
+      <c r="D27">
+        <v>4.8414677086223064</v>
+      </c>
+      <c r="E27">
+        <v>2.7525992868114462</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28">
+        <v>3.3851856329276453</v>
+      </c>
+      <c r="D28">
+        <v>4.5211411619510438</v>
+      </c>
+      <c r="E28">
+        <v>2.7327911833609662</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D29">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E29">
+        <v>2.8156199455261199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>3.7306001186370801</v>
+      </c>
+      <c r="D30">
+        <v>5.9557499885559082</v>
+      </c>
+      <c r="E30">
+        <v>2.8156199455261199</v>
       </c>
     </row>
   </sheetData>
@@ -857,13 +2352,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D652CE67-6E4B-4FE1-8654-61E2469CC07D}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -871,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -879,9 +2374,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -891,30 +2453,277 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9930EC86-EFE6-4982-BC8D-29EAB688DC49}">
-  <dimension ref="A4:A16"/>
+  <dimension ref="A4:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>3.0555555559885761E-3</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0.31555555555598858</v>
+      </c>
+      <c r="H18">
+        <v>0.42194444444498913</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0.26694444444501642</v>
+      </c>
+      <c r="E19">
+        <v>0.37555555555604769</v>
+      </c>
+      <c r="F19">
+        <v>2.5277777778001109E-2</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0.55166666666707442</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -924,53 +2733,53 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8AAAA1-54CC-42B8-BE43-3499790002DE}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
       <c r="B1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>463.94020876777279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8.9554865455410155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45.248611111111117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
       <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9.7361111111206355</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -978,9 +2787,142 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>